<commit_message>
add fresh metadata sheet
</commit_message>
<xml_diff>
--- a/templates/dataplant/plant_source.xlsx
+++ b/templates/dataplant/plant_source.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dominikbrilhaus/github/nfdi4plants/SWATE_templates/templates/dataplant/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dominikbrilhaus/github/Brilator/Swate-templates/templates/dataplant/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C39C2A4-8476-AB4C-B16C-ACCCBBD5BDC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34A1C515-0EDE-B346-9BA7-BA524FCE6F72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{B6C831B5-1971-5D49-B727-8B171A92DF3B}"/>
+    <workbookView xWindow="-17120" yWindow="-21100" windowWidth="27100" windowHeight="21100" activeTab="1" xr2:uid="{B6C831B5-1971-5D49-B727-8B171A92DF3B}"/>
   </bookViews>
   <sheets>
     <sheet name="plant_source" sheetId="1" r:id="rId1"/>
-    <sheet name="SwateTemplateMetadata" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="27">
   <si>
     <t>Source Name</t>
   </si>
@@ -42,87 +42,6 @@
     <t>Sample Name</t>
   </si>
   <si>
-    <t>Id</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Version</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Organisation</t>
-  </si>
-  <si>
-    <t>Table</t>
-  </si>
-  <si>
-    <t>#ER list</t>
-  </si>
-  <si>
-    <t>ER</t>
-  </si>
-  <si>
-    <t>ER Term Accession Number</t>
-  </si>
-  <si>
-    <t>ER Term Source REF</t>
-  </si>
-  <si>
-    <t>#TAGS list</t>
-  </si>
-  <si>
-    <t>Tags</t>
-  </si>
-  <si>
-    <t>Tags Term Accession Number</t>
-  </si>
-  <si>
-    <t>Tags Term Source REF</t>
-  </si>
-  <si>
-    <t>#AUTHORS list</t>
-  </si>
-  <si>
-    <t>Authors Last Name</t>
-  </si>
-  <si>
-    <t>Authors First Name</t>
-  </si>
-  <si>
-    <t>Authors Mid Initials</t>
-  </si>
-  <si>
-    <t>Authors Email</t>
-  </si>
-  <si>
-    <t>Authors Phone</t>
-  </si>
-  <si>
-    <t>Authors Fax</t>
-  </si>
-  <si>
-    <t>Authors Address</t>
-  </si>
-  <si>
-    <t>Authors Affiliation</t>
-  </si>
-  <si>
-    <t>Authors ORCID</t>
-  </si>
-  <si>
-    <t>Authors Role</t>
-  </si>
-  <si>
-    <t>Authors Role Term Accession Number</t>
-  </si>
-  <si>
-    <t>Authors Role Term Source REF</t>
-  </si>
-  <si>
     <t>02f15f9b-0a74-45b4-984c-47a1299b21c3</t>
   </si>
   <si>
@@ -181,6 +100,21 @@
   </si>
   <si>
     <t>Dominik</t>
+  </si>
+  <si>
+    <t>CEPLAS</t>
+  </si>
+  <si>
+    <t>https://orcid.org/0000-0001-9021-3197</t>
+  </si>
+  <si>
+    <t>plants</t>
+  </si>
+  <si>
+    <t>plant material</t>
+  </si>
+  <si>
+    <t>plant samples</t>
   </si>
 </sst>
 </file>
@@ -196,26 +130,20 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="12"/>
-      <color rgb="FFF5F5F5"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF217346"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -236,43 +164,12 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="4">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFFEFEFE"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FFFEFEFE"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFFEFEFE"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFFEFEFE"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FFFEFEFE"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -315,41 +212,34 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="12">
@@ -756,7 +646,7 @@
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -782,79 +672,79 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="D1" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="E1" t="s">
-        <v>36</v>
+        <v>9</v>
       </c>
       <c r="F1" t="s">
-        <v>37</v>
+        <v>10</v>
       </c>
       <c r="G1" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="H1" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="I1" t="s">
-        <v>40</v>
+        <v>13</v>
       </c>
       <c r="J1" t="s">
-        <v>41</v>
+        <v>14</v>
       </c>
       <c r="K1" t="s">
-        <v>42</v>
+        <v>15</v>
       </c>
       <c r="L1" t="s">
-        <v>43</v>
+        <v>16</v>
       </c>
       <c r="M1" t="s">
-        <v>44</v>
+        <v>17</v>
       </c>
       <c r="N1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B2" s="10"/>
-      <c r="C2" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="I2" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="J2" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="K2" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="L2" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="M2" s="10" t="s">
-        <v>33</v>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -866,196 +756,126 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{033823D9-457D-E64C-9751-88DF03A1D46B}">
-  <dimension ref="A1:B27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAA9F281-B02B-CC4F-8A09-E5DF2AE533E2}">
+  <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection sqref="A1:C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="32.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.5" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="1"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="2"/>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="5"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="6"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="2"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="2"/>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="5"/>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="2"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="3"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="1"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="1"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="2"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="6"/>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="2"/>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" s="2"/>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="5"/>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="1"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="1"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="2"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" s="2"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="2"/>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="2"/>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" s="1"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" s="1"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" s="1"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" s="1"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" s="1"/>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="2"/>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="2"/>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B23" s="2"/>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B24" s="2"/>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B25" s="2"/>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B26" s="2"/>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B27" s="8"/>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" s="1"/>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" s="1"/>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" s="4"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A24" r:id="rId1" xr:uid="{83CA1374-0188-5441-BA66-70FE2B4EF075}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>